<commit_message>
change idex_alu_op of tgeu/tgeiu/tltu/tltiu instruction. ---zheng bin
</commit_message>
<xml_diff>
--- a/doc/流水线CPU译码器信号表2.xlsx
+++ b/doc/流水线CPU译码器信号表2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="187">
   <si>
     <t>指令类型</t>
   </si>
@@ -832,6 +832,18 @@
   </si>
   <si>
     <t>01</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>0111</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>0111</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>0111</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -1782,10 +1794,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG77"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A82" sqref="A82"/>
-      <selection pane="topRight" activeCell="W73" sqref="W73"/>
+      <selection pane="topRight" activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -4797,8 +4809,8 @@
       <c r="J38" s="38">
         <v>0</v>
       </c>
-      <c r="K38" s="4" t="s">
-        <v>39</v>
+      <c r="K38" s="57" t="s">
+        <v>184</v>
       </c>
       <c r="L38" s="23"/>
       <c r="M38" s="24"/>
@@ -4872,8 +4884,8 @@
       <c r="J39" s="38">
         <v>1</v>
       </c>
-      <c r="K39" s="4" t="s">
-        <v>39</v>
+      <c r="K39" s="57" t="s">
+        <v>185</v>
       </c>
       <c r="L39" s="23"/>
       <c r="M39" s="24"/>
@@ -5097,8 +5109,8 @@
       <c r="J42" s="38">
         <v>0</v>
       </c>
-      <c r="K42" s="4" t="s">
-        <v>39</v>
+      <c r="K42" s="57" t="s">
+        <v>184</v>
       </c>
       <c r="L42" s="23"/>
       <c r="M42" s="24"/>
@@ -5172,8 +5184,8 @@
       <c r="J43" s="38">
         <v>1</v>
       </c>
-      <c r="K43" s="4" t="s">
-        <v>39</v>
+      <c r="K43" s="57" t="s">
+        <v>186</v>
       </c>
       <c r="L43" s="23"/>
       <c r="M43" s="24"/>

</xml_diff>